<commit_message>
ref #2 Updated Documentation
</commit_message>
<xml_diff>
--- a/docs/Sprint_C_Avaliacao_Interpares_3DC_G15.xlsx
+++ b/docs/Sprint_C_Avaliacao_Interpares_3DC_G15.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\LAPR5_3DC_G15\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A5FAC8F-D342-4231-83F0-ACABC064ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C87632A-AB7F-426E-907D-08A6411BA755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="F13" s="18">
         <f>AVERAGE(F10:F12)</f>
-        <v>2.3333333333333335</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1166,6 +1166,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -1349,22 +1364,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1380,28 +1404,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
closes #2 Final Commit
</commit_message>
<xml_diff>
--- a/docs/Sprint_C_Avaliacao_Interpares_3DC_G15.xlsx
+++ b/docs/Sprint_C_Avaliacao_Interpares_3DC_G15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\LAPR5_3DC_G15\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C87632A-AB7F-426E-907D-08A6411BA755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F03142B-8042-421C-928E-46BD5B4467F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="F13" s="18">
         <f>AVERAGE(F10:F12)</f>
-        <v>2.6666666666666665</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1166,21 +1166,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -1364,31 +1349,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1404,4 +1380,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>